<commit_message>
feat(pinmux_analysis): alpha version finish
</commit_message>
<xml_diff>
--- a/sample/pinmux.xlsx
+++ b/sample/pinmux.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="工作表2" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Pinmux" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -224,6 +225,7 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -337,79 +339,79 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -596,6 +598,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"頁 &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -603,16 +628,16 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H19" activeCellId="0" sqref="H19"/>
+      <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="3.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="3.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="3.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="27.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.25"/>
@@ -633,49 +658,49 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+    <row r="3" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
         <f aca="false">SUM(A6:A18)</f>
         <v>12</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" s="6" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="7" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" s="7" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="E5" s="9"/>
+    <row r="5" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="n">
+      <c r="A6" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -687,14 +712,14 @@
       <c r="E6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="H6" s="10"/>
-      <c r="K6" s="10" t="s">
+      <c r="F6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="K6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="n">
+      <c r="A7" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -706,14 +731,14 @@
       <c r="E7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="H7" s="10"/>
-      <c r="K7" s="10" t="s">
+      <c r="F7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="K7" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="n">
+      <c r="A8" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -725,14 +750,14 @@
       <c r="E8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="H8" s="10"/>
-      <c r="K8" s="10" t="s">
+      <c r="F8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="K8" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="n">
+      <c r="A9" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -744,14 +769,14 @@
       <c r="E9" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="H9" s="10"/>
-      <c r="K9" s="10" t="s">
+      <c r="F9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="K9" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="n">
+      <c r="A10" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -763,14 +788,14 @@
       <c r="E10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="5"/>
-      <c r="H10" s="10"/>
-      <c r="K10" s="10" t="s">
+      <c r="F10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="K10" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
+      <c r="A11" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -782,14 +807,14 @@
       <c r="E11" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="H11" s="10"/>
-      <c r="K11" s="10" t="s">
+      <c r="F11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="K11" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="n">
+      <c r="A12" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -801,19 +826,19 @@
       <c r="E12" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="6"/>
       <c r="H12" s="15" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="n">
+      <c r="A13" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -825,19 +850,19 @@
       <c r="E13" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="6"/>
       <c r="H13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="n">
+      <c r="A14" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -849,19 +874,19 @@
       <c r="E14" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="6"/>
       <c r="H14" s="15" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="n">
+      <c r="A15" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -873,19 +898,19 @@
       <c r="E15" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="6"/>
       <c r="H15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="n">
+      <c r="A16" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -897,14 +922,14 @@
       <c r="E16" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="H16" s="10"/>
-      <c r="K16" s="10" t="s">
+      <c r="F16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="K16" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="17" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="n">
+      <c r="A17" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -916,66 +941,66 @@
       <c r="E17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="H17" s="10"/>
-      <c r="K17" s="10" t="s">
+      <c r="F17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="K17" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="18" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="n">
+      <c r="A18" s="6" t="n">
         <v>0</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="F18" s="5"/>
-      <c r="H18" s="10"/>
-      <c r="K18" s="10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="n">
+      <c r="D18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="K18" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="n">
         <f aca="false">SUM(A23:A30)</f>
         <v>8</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" s="6" customFormat="true" ht="25.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="7" t="s">
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" s="7" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="7" t="s">
+      <c r="J21" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="7" t="s">
+      <c r="K21" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" s="8" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="n">
+    <row r="22" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -988,12 +1013,12 @@
       <c r="E23" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="K23" s="10" t="s">
+      <c r="K23" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="n">
+    <row r="24" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B24" s="17" t="s">
@@ -1006,12 +1031,12 @@
       <c r="E24" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="K24" s="10" t="s">
+      <c r="K24" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="n">
+    <row r="25" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B25" s="17" t="s">
@@ -1024,12 +1049,12 @@
       <c r="E25" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="10" t="s">
+      <c r="K25" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="n">
+    <row r="26" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -1042,12 +1067,12 @@
       <c r="E26" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="K26" s="10" t="s">
+      <c r="K26" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="n">
+    <row r="27" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B27" s="17" t="s">
@@ -1060,12 +1085,12 @@
       <c r="E27" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="10" t="s">
+      <c r="K27" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="n">
+    <row r="28" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B28" s="17" t="s">
@@ -1078,12 +1103,12 @@
       <c r="E28" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="K28" s="10" t="s">
+      <c r="K28" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="n">
+    <row r="29" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B29" s="17" t="s">
@@ -1096,12 +1121,12 @@
       <c r="E29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="6" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="n">
+    <row r="30" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="n">
         <v>1</v>
       </c>
       <c r="B30" s="17" t="s">
@@ -1114,7 +1139,7 @@
       <c r="E30" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="6" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
refactor(pinmux_analysis): JSON format refactor
</commit_message>
<xml_diff>
--- a/sample/pinmux.xlsx
+++ b/sample/pinmux.xlsx
@@ -220,27 +220,36 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
+    <font>
+      <sz val="12"/>
+      <name val="Noto Sans TC"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="136"/>
+    </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="9">
@@ -334,7 +343,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,11 +356,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -367,8 +380,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -379,7 +396,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,23 +404,27 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -411,7 +432,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -600,7 +621,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
@@ -623,12 +644,12 @@
   </sheetPr>
   <dimension ref="A2:K30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -648,498 +669,498 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="n">
+    <row r="3" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="n">
         <f aca="false">SUM(A6:A18)</f>
         <v>12</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="8" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" s="8" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="11" t="s">
+    <row r="5" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="K6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="F6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="K6" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="K7" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B8" s="11" t="s">
+      <c r="F7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="K7" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="K8" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="F8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="K8" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="K9" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="11" t="s">
+      <c r="F9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="K9" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="K10" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="11" t="s">
+      <c r="F10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="K10" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="K11" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
+      <c r="F11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="K11" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="H12" s="15" t="s">
+      <c r="F12" s="7"/>
+      <c r="H12" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="16" t="s">
+      <c r="I12" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="11" t="s">
+      <c r="K12" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="H13" s="15" t="s">
+      <c r="F13" s="7"/>
+      <c r="H13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="I13" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="11" t="s">
+      <c r="K13" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="H14" s="15" t="s">
+      <c r="F14" s="7"/>
+      <c r="H14" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" s="11" t="s">
+      <c r="K14" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E15" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="6"/>
-      <c r="H15" s="15" t="s">
+      <c r="F15" s="7"/>
+      <c r="H15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="11" t="s">
+      <c r="K15" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="K16" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="11" t="s">
+      <c r="F16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="K16" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="K17" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" s="12" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6" t="n">
+      <c r="F17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="K17" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="K18" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="n">
+      <c r="D18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="K18" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="n">
         <f aca="false">SUM(A23:A30)</f>
         <v>8</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" s="7" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="8" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" s="8" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="8" t="s">
+      <c r="J21" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="K21" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" s="17" t="s">
+    <row r="22" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="18"/>
-      <c r="D23" s="13" t="s">
+      <c r="C23" s="21"/>
+      <c r="D23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B24" s="17" t="s">
+    <row r="24" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="21"/>
+      <c r="D24" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E24" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="K24" s="6" t="s">
+      <c r="K24" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B25" s="17" t="s">
+    <row r="25" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="18"/>
-      <c r="D25" s="13" t="s">
+      <c r="C25" s="21"/>
+      <c r="D25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="K25" s="6" t="s">
+      <c r="K25" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B26" s="17" t="s">
+    <row r="26" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="18"/>
-      <c r="D26" s="13" t="s">
+      <c r="C26" s="21"/>
+      <c r="D26" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="K26" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B27" s="17" t="s">
+    <row r="27" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="18"/>
-      <c r="D27" s="13" t="s">
+      <c r="C27" s="21"/>
+      <c r="D27" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="K27" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B28" s="17" t="s">
+    <row r="28" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="18"/>
-      <c r="D28" s="13" t="s">
+      <c r="C28" s="21"/>
+      <c r="D28" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="19" t="s">
+      <c r="E28" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="K28" s="6" t="s">
+      <c r="K28" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B29" s="17" t="s">
+    <row r="29" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="13" t="s">
+      <c r="C29" s="21"/>
+      <c r="D29" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="19" t="s">
+      <c r="E29" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="B30" s="17" t="s">
+    <row r="30" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="13" t="s">
+      <c r="C30" s="21"/>
+      <c r="D30" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="K30" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1148,8 +1169,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;10&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;10頁 &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Arial,標準"&amp;10&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Arial,標準"&amp;10頁 &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(pinmux_analysis): support partition mode
</commit_message>
<xml_diff>
--- a/sample/pinmux.xlsx
+++ b/sample/pinmux.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
     <t xml:space="preserve">Function 1</t>
   </si>
@@ -211,6 +211,33 @@
   </si>
   <si>
     <t xml:space="preserve">FUNC_INOUT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGPIO1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG_TCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAD TYPE2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGPIO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG_TMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGPIO3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG_TDI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DGPIO4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JTAG_TDO</t>
   </si>
 </sst>
 </file>
@@ -231,19 +258,16 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="136"/>
     </font>
     <font>
       <sz val="12"/>
@@ -360,7 +384,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -625,7 +649,7 @@
       <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.62890625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -642,17 +666,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K30"/>
+  <dimension ref="A2:K38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E32" activeCellId="0" sqref="E32"/>
+      <selection pane="bottomRight" activeCell="K39" activeCellId="0" sqref="K39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.640625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.34375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="16.24"/>
@@ -663,9 +687,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="27.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="27.07"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.65"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="9.64"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
         <f aca="false">SUM(A6:A18)</f>
         <v>12</v>
@@ -694,17 +717,24 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-    </row>
-    <row r="4" s="8" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+    </row>
+    <row r="4" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8"/>
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="8"/>
       <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
       <c r="I4" s="10" t="s">
         <v>7</v>
       </c>
@@ -715,18 +745,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="11"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
+      <c r="D5" s="11"/>
       <c r="E5" s="12"/>
-    </row>
-    <row r="6" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
+      <c r="C6" s="14"/>
       <c r="D6" s="15" t="s">
         <v>11</v>
       </c>
@@ -734,18 +773,22 @@
         <v>12</v>
       </c>
       <c r="F6" s="7"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="7"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
+      <c r="C7" s="14"/>
       <c r="D7" s="15" t="s">
         <v>15</v>
       </c>
@@ -753,18 +796,22 @@
         <v>16</v>
       </c>
       <c r="F7" s="7"/>
+      <c r="G7" s="14"/>
       <c r="H7" s="7"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="C8" s="14"/>
       <c r="D8" s="15" t="s">
         <v>15</v>
       </c>
@@ -772,18 +819,22 @@
         <v>18</v>
       </c>
       <c r="F8" s="7"/>
+      <c r="G8" s="14"/>
       <c r="H8" s="7"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>19</v>
       </c>
+      <c r="C9" s="14"/>
       <c r="D9" s="15" t="s">
         <v>15</v>
       </c>
@@ -791,18 +842,22 @@
         <v>20</v>
       </c>
       <c r="F9" s="7"/>
+      <c r="G9" s="14"/>
       <c r="H9" s="7"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
       <c r="K9" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>21</v>
       </c>
+      <c r="C10" s="14"/>
       <c r="D10" s="15" t="s">
         <v>15</v>
       </c>
@@ -810,18 +865,22 @@
         <v>22</v>
       </c>
       <c r="F10" s="7"/>
+      <c r="G10" s="14"/>
       <c r="H10" s="7"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
       <c r="K10" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="C11" s="14"/>
       <c r="D11" s="15" t="s">
         <v>15</v>
       </c>
@@ -829,18 +888,22 @@
         <v>24</v>
       </c>
       <c r="F11" s="7"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="7"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
       <c r="K11" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>25</v>
       </c>
+      <c r="C12" s="14"/>
       <c r="D12" s="18" t="s">
         <v>11</v>
       </c>
@@ -848,23 +911,26 @@
         <v>26</v>
       </c>
       <c r="F12" s="7"/>
+      <c r="G12" s="14"/>
       <c r="H12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="19" t="s">
         <v>27</v>
       </c>
+      <c r="J12" s="14"/>
       <c r="K12" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
+      <c r="C13" s="14"/>
       <c r="D13" s="18" t="s">
         <v>15</v>
       </c>
@@ -872,23 +938,26 @@
         <v>29</v>
       </c>
       <c r="F13" s="7"/>
+      <c r="G13" s="14"/>
       <c r="H13" s="18" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>30</v>
       </c>
+      <c r="J13" s="14"/>
       <c r="K13" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>31</v>
       </c>
+      <c r="C14" s="14"/>
       <c r="D14" s="18" t="s">
         <v>15</v>
       </c>
@@ -896,23 +965,26 @@
         <v>32</v>
       </c>
       <c r="F14" s="7"/>
+      <c r="G14" s="14"/>
       <c r="H14" s="18" t="s">
         <v>33</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>34</v>
       </c>
+      <c r="J14" s="14"/>
       <c r="K14" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B15" s="13" t="s">
         <v>35</v>
       </c>
+      <c r="C15" s="14"/>
       <c r="D15" s="18" t="s">
         <v>15</v>
       </c>
@@ -920,23 +992,26 @@
         <v>36</v>
       </c>
       <c r="F15" s="7"/>
+      <c r="G15" s="14"/>
       <c r="H15" s="18" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>37</v>
       </c>
+      <c r="J15" s="14"/>
       <c r="K15" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>38</v>
       </c>
+      <c r="C16" s="14"/>
       <c r="D16" s="18" t="s">
         <v>15</v>
       </c>
@@ -944,18 +1019,22 @@
         <v>39</v>
       </c>
       <c r="F16" s="7"/>
+      <c r="G16" s="14"/>
       <c r="H16" s="7"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="n">
         <v>1</v>
       </c>
       <c r="B17" s="13" t="s">
         <v>40</v>
       </c>
+      <c r="C17" s="14"/>
       <c r="D17" s="18" t="s">
         <v>15</v>
       </c>
@@ -963,26 +1042,34 @@
         <v>41</v>
       </c>
       <c r="F17" s="7"/>
+      <c r="G17" s="14"/>
       <c r="H17" s="7"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
       <c r="K17" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" s="14" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="n">
         <v>0</v>
       </c>
       <c r="B18" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="C18" s="14"/>
       <c r="D18" s="7"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="7"/>
+      <c r="G18" s="14"/>
       <c r="H18" s="7"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
       <c r="K18" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
         <f aca="false">SUM(A23:A30)</f>
         <v>8</v>
@@ -997,17 +1084,25 @@
       <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
-    </row>
-    <row r="21" s="8" customFormat="true" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8"/>
       <c r="B21" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="D21" s="8"/>
       <c r="E21" s="9" t="s">
         <v>44</v>
       </c>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
       <c r="J21" s="9" t="s">
         <v>8</v>
       </c>
@@ -1015,12 +1110,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="11"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="12"/>
-    </row>
-    <row r="23" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="n">
         <v>1</v>
       </c>
@@ -1034,11 +1137,16 @@
       <c r="E23" s="22" t="s">
         <v>46</v>
       </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
       <c r="K23" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="n">
         <v>1</v>
       </c>
@@ -1052,11 +1160,16 @@
       <c r="E24" s="22" t="s">
         <v>49</v>
       </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="n">
         <v>1</v>
       </c>
@@ -1070,11 +1183,16 @@
       <c r="E25" s="22" t="s">
         <v>51</v>
       </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
       <c r="K25" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="n">
         <v>1</v>
       </c>
@@ -1088,11 +1206,16 @@
       <c r="E26" s="22" t="s">
         <v>53</v>
       </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
       <c r="K26" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="27" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="7" t="n">
         <v>1</v>
       </c>
@@ -1106,11 +1229,16 @@
       <c r="E27" s="22" t="s">
         <v>55</v>
       </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
       <c r="K27" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="28" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="7" t="n">
         <v>1</v>
       </c>
@@ -1124,11 +1252,16 @@
       <c r="E28" s="22" t="s">
         <v>57</v>
       </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
       <c r="K28" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="7" t="n">
         <v>1</v>
       </c>
@@ -1142,11 +1275,16 @@
       <c r="E29" s="22" t="s">
         <v>59</v>
       </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
       <c r="K29" s="17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="30" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="7" t="n">
         <v>1</v>
       </c>
@@ -1160,8 +1298,159 @@
       <c r="E30" s="22" t="s">
         <v>61</v>
       </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
       <c r="K30" s="17" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="4" t="n">
+        <f aca="false">SUM(A35:A43)</f>
+        <v>4</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="8"/>
+      <c r="B33" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="21"/>
+      <c r="D35" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="21"/>
+      <c r="D36" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="21"/>
+      <c r="D37" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="21"/>
+      <c r="D38" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="17" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>